<commit_message>
modify static anlaysis format
</commit_message>
<xml_diff>
--- a/static analysis/정적분석포맷.xlsx
+++ b/static analysis/정적분석포맷.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\연구와 레포지토리\vnv-team-3\static analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3862F8-7D2B-4B9A-B0BB-9080FCA813CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E87685-292F-4FF1-BF94-17C7DDB52079}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F6AB2B5B-B36D-48D8-B551-DDFE101EE59E}"/>
   </bookViews>
@@ -134,10 +134,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>에러의 설명을 간단히 기입해줍니다. 젠킨스 보고서에 영어로 잘 설명되어 있습니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>에러를 일으킨 코드 위치를 밝혀 줍니다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -326,6 +322,10 @@
   </si>
   <si>
     <t>equals()를 호출하세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에러의 설명을 간단히 기입해줍니다. '중요한 에러' 탭의 에러 설명을 그대로 사용.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -452,6 +452,21 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,21 +480,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -799,7 +799,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -808,40 +808,40 @@
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="8">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
       <c r="F3" t="s">
         <v>20</v>
       </c>
@@ -850,87 +850,87 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -954,7 +954,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -965,222 +965,222 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="11" spans="1:3" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>50</v>
-      </c>
-      <c r="C19" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
         <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>59</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
         <v>61</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>62</v>
-      </c>
-      <c r="C23" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
         <v>64</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>65</v>
-      </c>
-      <c r="C24" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
         <v>67</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>68</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>